<commit_message>
ADDED inputVal for dropdown
</commit_message>
<xml_diff>
--- a/src/Assets/templates/STAGE_PROCESSING_INV_TRAN_TEMPLATE.xlsx
+++ b/src/Assets/templates/STAGE_PROCESSING_INV_TRAN_TEMPLATE.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Downloads/Inventory_&amp;_Non_Inventory_TRN_TYPE_Drop_Down/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\26-08-2022 screens\src\Assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2D92A6-423D-744A-AB07-386819130C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23380" windowHeight="13720" xr2:uid="{D11E406A-9774-4019-9D76-799F1FD67D66}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -90,12 +89,6 @@
     <t>Cost Variance</t>
   </si>
   <si>
-    <t>Inventory Ajustment</t>
-  </si>
-  <si>
-    <t>Inventory Ajustment COGS</t>
-  </si>
-  <si>
     <t>Deal Income Sales</t>
   </si>
   <si>
@@ -178,12 +171,18 @@
   </si>
   <si>
     <t>LOC</t>
+  </si>
+  <si>
+    <t>Inventory Adjustment</t>
+  </si>
+  <si>
+    <t>Inventory Adjustment COGS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -290,10 +289,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4ECD93D8-1268-4144-82F3-A4DA85A96514}" name="Table1" displayName="Table1" ref="A2:A37" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A2:A37" xr:uid="{4ECD93D8-1268-4144-82F3-A4DA85A96514}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:A37" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A2:A37"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{9D77BE92-133A-4C44-A3FB-1A1307FFAF21}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="1" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -595,37 +594,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34911EF7-C436-4C00-98DA-269DAE10883F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="8.5" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" customWidth="1"/>
-    <col min="12" max="12" width="10.5" customWidth="1"/>
+    <col min="1" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -661,7 +660,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid TRN_TYPE !" error="The TRN_TYPE you have entered is invalid. Please select the correct value to continue." promptTitle="TRN_TYPE" prompt="Please select a TRN_TYPE from the list." xr:uid="{BE6C7203-03B2-413E-8585-D2BB54D54299}">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid TRN_TYPE !" error="The TRN_TYPE you have entered is invalid. Please select the correct value to continue." promptTitle="TRN_TYPE" prompt="Please select a TRN_TYPE from the list.">
           <x14:formula1>
             <xm:f>Sheet1!$A$3:$A$17</xm:f>
           </x14:formula1>
@@ -674,21 +673,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B19BDEF-E4D8-4A8B-A85D-D217A1FC58C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C22"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="38.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="38.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -696,191 +695,191 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="4" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="4" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="C18" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="C19" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="C20" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="C21" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="C22" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
     </row>
   </sheetData>

</xml_diff>